<commit_message>
added positional and salary data
</commit_message>
<xml_diff>
--- a/data/arizona.xlsx
+++ b/data/arizona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clint\Documents\nss\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE71304-567C-4602-8824-273E57EDFCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7408AFB6-DC49-46A3-9C58-2238BFC22E9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" activeTab="9" xr2:uid="{088C41B1-79EA-425F-8A1D-814996B19A9A}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" firstSheet="1" activeTab="3" xr2:uid="{088C41B1-79EA-425F-8A1D-814996B19A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="2011" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="2018" sheetId="8" r:id="rId8"/>
     <sheet name="2019" sheetId="9" r:id="rId9"/>
     <sheet name="2020" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3177" uniqueCount="424">
   <si>
     <t>Player </t>
   </si>
@@ -1291,6 +1292,21 @@
   </si>
   <si>
     <t>J.R. Sweezy</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>MLB</t>
+  </si>
+  <si>
+    <t>G-T</t>
+  </si>
+  <si>
+    <t>TE</t>
   </si>
 </sst>
 </file>
@@ -2149,88 +2165,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E499E39-B74F-4EC9-B8F3-F7914F0EB626}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="B2" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2243,19 +2265,24 @@
       <c r="N2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="O2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>421</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2264,23 +2291,26 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>422</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2289,26 +2319,27 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B5" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>24</v>
@@ -2349,12 +2380,17 @@
       <c r="Q5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="R5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="5" t="s">
+        <v>420</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2366,9 +2402,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
         <v>23</v>
       </c>
@@ -2376,14 +2410,17 @@
         <v>23</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+        <v>23</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2393,33 +2430,34 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -2428,20 +2466,21 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
+      <c r="B9" s="5" t="s">
+        <v>423</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
@@ -2452,12 +2491,14 @@
         <v>23</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2465,22 +2506,23 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -2488,12 +2530,13 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-    </row>
-    <row r="11" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2506,100 +2549,105 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="Q11" s="2"/>
-    </row>
-    <row r="12" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="5" t="s">
+        <v>423</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I12" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="L13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="Q13" s="2"/>
-    </row>
-    <row r="14" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2610,12 +2658,13 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-    </row>
-    <row r="15" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2629,122 +2678,126 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+        <v>19</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="O16" s="2"/>
       <c r="P16" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+        <v>23</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="K17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="M17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="2"/>
       <c r="P17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-    </row>
-    <row r="19" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2759,12 +2812,13 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2779,30 +2833,29 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-      <c r="Q20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="E21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>23</v>
@@ -2817,33 +2870,34 @@
         <v>23</v>
       </c>
       <c r="M21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="O21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
         <v>23</v>
       </c>
@@ -2866,62 +2920,66 @@
         <v>23</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+        <v>23</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="O23" s="2"/>
       <c r="P23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+        <v>23</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2932,42 +2990,44 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-    </row>
-    <row r="25" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="2"/>
+      <c r="L25" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-    </row>
-    <row r="26" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="2"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2982,15 +3042,16 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="2"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -3003,31 +3064,30 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="P27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
         <v>19</v>
       </c>
@@ -3040,31 +3100,34 @@
       <c r="M28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="O28" s="2"/>
-      <c r="P28" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="P28" s="2"/>
       <c r="Q28" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+        <v>19</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -3075,14 +3138,13 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B30" s="5"/>
       <c r="C30" s="2" t="s">
         <v>24</v>
       </c>
@@ -3128,12 +3190,15 @@
       <c r="Q30" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -3144,26 +3209,27 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="1:18" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -3176,27 +3242,26 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-    </row>
-    <row r="33" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R32" s="2"/>
+    </row>
+    <row r="33" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
         <v>19</v>
       </c>
@@ -3218,13 +3283,16 @@
       <c r="P33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="2"/>
-    </row>
-    <row r="34" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="Q33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -3234,9 +3302,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="L34" s="2"/>
       <c r="M34" s="2" t="s">
         <v>24</v>
       </c>
@@ -3252,14 +3318,15 @@
       <c r="Q34" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B35" s="5"/>
       <c r="C35" s="2" t="s">
         <v>24</v>
       </c>
@@ -3305,15 +3372,18 @@
       <c r="Q35" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="2"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3328,14 +3398,13 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
-    </row>
-    <row r="37" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B37" s="5"/>
       <c r="C37" s="2" t="s">
         <v>24</v>
       </c>
@@ -3381,39 +3450,43 @@
       <c r="Q37" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="R37" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="2"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E38" s="2"/>
-      <c r="F38" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
-      <c r="N38" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="N38" s="2"/>
       <c r="O38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q38" s="2"/>
+      <c r="Q38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3424,8 +3497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F078A4-76EF-4A08-A28D-1604CAF29724}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4078,6 +4151,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551B41FD-C427-44E1-BC4E-E880F7C43676}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6500,8 +6586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53863249-B0CA-41AB-B335-C4A2CF671AC3}">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -7640,11 +7726,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD01725E-0FAF-4F8D-A038-2808722E5EBC}">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B20" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="16.2265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -8759,6 +8848,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8766,11 +8856,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06D11DD-8291-46D3-B50F-DB4A755A81ED}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B14" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="15.04296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -9741,11 +9834,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED8CE35-81EF-4F5E-A409-6A32DE24DE21}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B19" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="20.1328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -10870,11 +10966,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEB50E7-10B4-4790-9E58-BAE93821AFC9}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B28" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
@@ -10982,7 +11081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="3" t="s">
         <v>306</v>
       </c>
@@ -11009,7 +11108,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" s="3" t="s">
         <v>307</v>
       </c>
@@ -11042,7 +11141,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="3" t="s">
         <v>308</v>
       </c>
@@ -11065,7 +11164,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A6" s="3" t="s">
         <v>309</v>
       </c>
@@ -11092,7 +11191,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="3" t="s">
         <v>168</v>
       </c>
@@ -11121,7 +11220,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" s="3" t="s">
         <v>275</v>
       </c>
@@ -11205,7 +11304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" s="3" t="s">
         <v>311</v>
       </c>
@@ -11258,7 +11357,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="3" t="s">
         <v>312</v>
       </c>
@@ -11281,7 +11380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
         <v>313</v>
       </c>
@@ -11341,7 +11440,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="3" t="s">
         <v>83</v>
       </c>
@@ -11368,7 +11467,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A15" s="3" t="s">
         <v>315</v>
       </c>
@@ -11537,7 +11636,7 @@
       </c>
       <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A20" s="3" t="s">
         <v>318</v>
       </c>
@@ -11560,7 +11659,7 @@
       </c>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A21" s="3" t="s">
         <v>245</v>
       </c>
@@ -11597,7 +11696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A22" s="3" t="s">
         <v>210</v>
       </c>
@@ -11638,7 +11737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A23" s="3" t="s">
         <v>319</v>
       </c>
@@ -11667,7 +11766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A24" s="3" t="s">
         <v>279</v>
       </c>
@@ -11690,7 +11789,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A25" s="3" t="s">
         <v>249</v>
       </c>
@@ -11743,7 +11842,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A26" s="3" t="s">
         <v>320</v>
       </c>
@@ -11819,7 +11918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A28" s="3" t="s">
         <v>322</v>
       </c>
@@ -11895,7 +11994,7 @@
       </c>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A30" s="3" t="s">
         <v>253</v>
       </c>
@@ -11987,7 +12086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A32" s="3" t="s">
         <v>217</v>
       </c>
@@ -12041,7 +12140,7 @@
       </c>
       <c r="Q33" s="4"/>
     </row>
-    <row r="34" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A34" s="3" t="s">
         <v>324</v>
       </c>
@@ -12064,7 +12163,7 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
     </row>
-    <row r="35" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A35" s="3" t="s">
         <v>283</v>
       </c>
@@ -12103,7 +12202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A36" s="3" t="s">
         <v>325</v>
       </c>
@@ -12169,7 +12268,7 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
-    <row r="38" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A38" s="3" t="s">
         <v>327</v>
       </c>
@@ -12194,7 +12293,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A39" s="3" t="s">
         <v>284</v>
       </c>
@@ -12247,7 +12346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A40" s="3" t="s">
         <v>328</v>
       </c>
@@ -12276,7 +12375,7 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
     </row>
-    <row r="41" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A41" s="3" t="s">
         <v>329</v>
       </c>
@@ -12301,7 +12400,7 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
     </row>
-    <row r="42" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A42" s="3" t="s">
         <v>330</v>
       </c>
@@ -12338,7 +12437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A43" s="3" t="s">
         <v>285</v>
       </c>
@@ -12377,7 +12476,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A44" s="3" t="s">
         <v>286</v>
       </c>
@@ -12412,6 +12511,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12420,10 +12520,13 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="14.40625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="5" t="s">
@@ -12478,7 +12581,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A2" s="5" t="s">
         <v>346</v>
       </c>
@@ -12531,7 +12634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
         <v>347</v>
       </c>
@@ -12576,7 +12679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" s="5" t="s">
         <v>348</v>
       </c>
@@ -12603,7 +12706,7 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A5" s="5" t="s">
         <v>349</v>
       </c>
@@ -12663,7 +12766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A7" s="5" t="s">
         <v>351</v>
       </c>
@@ -12716,7 +12819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" s="5" t="s">
         <v>352</v>
       </c>
@@ -12743,7 +12846,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A9" s="5" t="s">
         <v>353</v>
       </c>
@@ -12766,7 +12869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" s="5" t="s">
         <v>354</v>
       </c>
@@ -12789,7 +12892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A11" s="5" t="s">
         <v>314</v>
       </c>
@@ -12816,7 +12919,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A12" s="5" t="s">
         <v>315</v>
       </c>
@@ -12886,7 +12989,7 @@
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A14" s="5" t="s">
         <v>356</v>
       </c>
@@ -12929,7 +13032,7 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A15" s="5" t="s">
         <v>316</v>
       </c>
@@ -12958,7 +13061,7 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A16" s="5" t="s">
         <v>358</v>
       </c>
@@ -13011,7 +13114,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A17" s="5" t="s">
         <v>317</v>
       </c>
@@ -13038,7 +13141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A18" s="5" t="s">
         <v>359</v>
       </c>
@@ -13061,7 +13164,7 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A19" s="5" t="s">
         <v>360</v>
       </c>
@@ -13084,7 +13187,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A20" s="5" t="s">
         <v>212</v>
       </c>
@@ -13113,7 +13216,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A21" s="5" t="s">
         <v>361</v>
       </c>
@@ -13161,7 +13264,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A23" s="5" t="s">
         <v>319</v>
       </c>
@@ -13221,7 +13324,7 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A25" s="5" t="s">
         <v>364</v>
       </c>
@@ -13256,7 +13359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A26" s="5" t="s">
         <v>365</v>
       </c>
@@ -13279,7 +13382,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A27" s="5" t="s">
         <v>366</v>
       </c>
@@ -13324,7 +13427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A28" s="5" t="s">
         <v>367</v>
       </c>
@@ -13347,7 +13450,7 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A29" s="5" t="s">
         <v>368</v>
       </c>
@@ -13374,7 +13477,7 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
     </row>
-    <row r="30" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A30" s="5" t="s">
         <v>369</v>
       </c>
@@ -13399,7 +13502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A31" s="5" t="s">
         <v>370</v>
       </c>
@@ -13422,7 +13525,7 @@
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A32" s="5" t="s">
         <v>371</v>
       </c>
@@ -13451,7 +13554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A33" s="5" t="s">
         <v>325</v>
       </c>
@@ -13478,7 +13581,7 @@
       </c>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A34" s="5" t="s">
         <v>326</v>
       </c>
@@ -13505,7 +13608,7 @@
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
     </row>
-    <row r="35" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A35" s="5" t="s">
         <v>372</v>
       </c>
@@ -13540,7 +13643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A36" s="5" t="s">
         <v>373</v>
       </c>
@@ -13563,7 +13666,7 @@
       </c>
       <c r="Q36" s="6"/>
     </row>
-    <row r="37" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A37" s="5" t="s">
         <v>374</v>
       </c>
@@ -13614,7 +13717,7 @@
       </c>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A38" s="5" t="s">
         <v>284</v>
       </c>
@@ -13637,7 +13740,7 @@
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A39" s="5" t="s">
         <v>375</v>
       </c>
@@ -13666,7 +13769,7 @@
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
     </row>
-    <row r="40" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A40" s="5" t="s">
         <v>376</v>
       </c>
@@ -13719,7 +13822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A41" s="5" t="s">
         <v>377</v>
       </c>
@@ -13744,7 +13847,7 @@
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
     </row>
-    <row r="42" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A42" s="5" t="s">
         <v>378</v>
       </c>
@@ -13767,7 +13870,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A43" s="5" t="s">
         <v>379</v>
       </c>
@@ -13790,7 +13893,7 @@
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A44" s="5" t="s">
         <v>380</v>
       </c>
@@ -13827,7 +13930,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A45" s="5" t="s">
         <v>381</v>
       </c>
@@ -13860,7 +13963,7 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A46" s="5" t="s">
         <v>382</v>
       </c>
@@ -13885,7 +13988,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A47" s="5" t="s">
         <v>383</v>
       </c>
@@ -13908,7 +14011,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
     </row>
-    <row r="48" spans="1:17" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A48" s="5" t="s">
         <v>384</v>
       </c>
@@ -13990,7 +14093,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A50" s="5" t="s">
         <v>385</v>
       </c>
@@ -14013,7 +14116,7 @@
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
     </row>
-    <row r="51" spans="1:17" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A51" s="5" t="s">
         <v>386</v>
       </c>

</xml_diff>